<commit_message>
marked COP as COP_h to clarify that it is computed as heating COP regardless of mode
</commit_message>
<xml_diff>
--- a/PythonResources/RunCases/cop_for_milp.xlsx
+++ b/PythonResources/RunCases/cop_for_milp.xlsx
@@ -38,7 +38,7 @@
     <t>simultaneous</t>
   </si>
   <si>
-    <t>COP_mon</t>
+    <t>COP_h</t>
   </si>
   <si>
     <t>Duration|h</t>
@@ -116,7 +116,7 @@
     <t>343b6a5a47399dbee9441f1aaf96fb83d38b8aa6</t>
   </si>
   <si>
-    <t>0a990b24df40bd895ee2096141ebc3be5eb0518b</t>
+    <t>8c9be2b139daaededa2449d96e69823138e0dd27</t>
   </si>
 </sst>
 </file>

</xml_diff>